<commit_message>
Added required fields to XLSX files. Amended the dataset_template.json file.
</commit_message>
<xml_diff>
--- a/datasets/dataset_values.xlsx
+++ b/datasets/dataset_values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/git/jsonld_templates/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF39F08D-B95F-774C-99E1-B3A9AABCF7F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8C9934-55EC-4444-89D1-5648C54D747B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="33600" windowHeight="18920" xr2:uid="{4CEDCFA5-5B2F-A948-BAD6-24B4F525AA04}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18940" xr2:uid="{4CEDCFA5-5B2F-A948-BAD6-24B4F525AA04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="51">
   <si>
     <t>Element</t>
   </si>
@@ -78,9 +78,6 @@
     <t>publisher</t>
   </si>
   <si>
-    <t>creator</t>
-  </si>
-  <si>
     <t>spatialCoverage</t>
   </si>
   <si>
@@ -166,6 +163,21 @@
   </si>
   <si>
     <t>MAIN</t>
+  </si>
+  <si>
+    <t>creator (person)</t>
+  </si>
+  <si>
+    <t>creator (role)</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -197,7 +209,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -263,11 +275,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -278,6 +305,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -594,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F6CA01-35FA-E247-89D4-281F1723A239}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="141" zoomScaleNormal="141" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,18 +639,18 @@
     <col min="5" max="5" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D1" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>1</v>
@@ -628,8 +658,11 @@
       <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -637,13 +670,16 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -651,13 +687,16 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -665,13 +704,16 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -679,13 +721,16 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -693,13 +738,16 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -707,13 +755,16 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -721,13 +772,16 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -735,13 +789,16 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -749,13 +806,16 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -763,13 +823,16 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -777,13 +840,16 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -791,13 +857,16 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -805,41 +874,50 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -847,13 +925,16 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>3</v>
@@ -861,27 +942,33 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>4</v>
@@ -889,13 +976,16 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -903,13 +993,16 @@
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -917,13 +1010,16 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>3</v>
@@ -931,13 +1027,16 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>7</v>
@@ -945,13 +1044,16 @@
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>4</v>
@@ -959,13 +1061,16 @@
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>6</v>
@@ -973,27 +1078,33 @@
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>3</v>
@@ -1001,27 +1112,33 @@
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>6</v>
@@ -1029,27 +1146,33 @@
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
@@ -1057,13 +1180,16 @@
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
@@ -1071,41 +1197,50 @@
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
@@ -1113,27 +1248,33 @@
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1141,41 +1282,50 @@
         <v>6</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>4</v>
@@ -1183,125 +1333,152 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
         <v>3</v>
@@ -1309,13 +1486,16 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>7</v>
@@ -1323,13 +1503,16 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
         <v>4</v>
@@ -1337,27 +1520,33 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
         <v>6</v>
@@ -1365,25 +1554,27 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G54" s="1"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G55" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>